<commit_message>
user request dashboard, takes in all request made by logged in user
</commit_message>
<xml_diff>
--- a/video-streaming.xlsx
+++ b/video-streaming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muath\Documents\webDev\video-streaming-platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68825E5-5F4E-429A-9116-C41BA5FC9C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6930F0DB-9CF0-44EA-B106-A03E1649052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D6F4BC0A-9AEB-4F25-B0EC-11787D3112BA}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -578,11 +578,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3" si="0">MROUND(B3, 0.5)</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -596,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C19" si="1">MROUND(B4, 0.5)</f>
+        <f t="shared" ref="C4:C19" si="0">MROUND(B4, 0.5)</f>
         <v>0</v>
       </c>
       <c r="D4" s="3">
@@ -611,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D5" s="3">
@@ -626,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D6" s="3">
@@ -641,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D7" s="3">
@@ -653,11 +652,11 @@
         <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -671,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9" s="3">
@@ -686,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D10" s="3">
@@ -698,10 +697,9 @@
         <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D11" s="3">
@@ -713,10 +711,9 @@
         <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D12" s="3">
@@ -731,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13" s="3">
@@ -746,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="3">
@@ -761,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D15" s="3">
@@ -772,12 +769,11 @@
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.8</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -791,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D17" s="3">
@@ -806,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D18" s="3">
@@ -821,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D19" s="3">
@@ -850,7 +846,7 @@
         <v>0.6</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" ref="C21" si="2">MROUND(B21, 0.5)</f>
+        <f t="shared" ref="C21" si="1">MROUND(B21, 0.5)</f>
         <v>0.5</v>
       </c>
       <c r="D21" s="3">

</xml_diff>